<commit_message>
Final Uploads for The Appendix
</commit_message>
<xml_diff>
--- a/Manually Compiled data/DescriptiveRepresentationStats.xlsx
+++ b/Manually Compiled data/DescriptiveRepresentationStats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b121ec5fbd34cca4/Documents/MA thesis/Data and R scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b121ec5fbd34cca4/Documents/MA thesis/MA-Thesis-Appendix/Manually Compiled data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1084" documentId="8_{A8720AE2-E0E9-4F8C-9739-CBADF2F7E248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C0402CA-4FF0-439A-B229-A3439AD8BFD2}"/>
+  <xr:revisionPtr revIDLastSave="1126" documentId="8_{A8720AE2-E0E9-4F8C-9739-CBADF2F7E248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C475E162-7591-458C-B603-F999D4B46FEC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE3C31C3-AAEA-42AF-B109-42DB1278F21B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{DE3C31C3-AAEA-42AF-B109-42DB1278F21B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
   <si>
     <t>TaiwanYear</t>
   </si>
@@ -128,21 +128,6 @@
     <t>Post-with-t</t>
   </si>
   <si>
-    <t>0.12213959</t>
-  </si>
-  <si>
-    <t>0.01943892</t>
-  </si>
-  <si>
-    <t>0.15028143</t>
-  </si>
-  <si>
-    <t>0.08699878</t>
-  </si>
-  <si>
-    <t>DiD Model</t>
-  </si>
-  <si>
     <t>DDD Model</t>
   </si>
   <si>
@@ -158,12 +143,6 @@
     <t>post-with-t</t>
   </si>
   <si>
-    <t>0.40083191†</t>
-  </si>
-  <si>
-    <t>0.02457844†</t>
-  </si>
-  <si>
     <t>95% CI</t>
   </si>
   <si>
@@ -218,15 +197,9 @@
     <t>8.66% †</t>
   </si>
   <si>
-    <t>8.76 % †</t>
-  </si>
-  <si>
     <t>18.6% †</t>
   </si>
   <si>
-    <t>9.66 % †</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -375,6 +348,63 @@
   </si>
   <si>
     <t>8.253e-15</t>
+  </si>
+  <si>
+    <t>Candidate Model</t>
+  </si>
+  <si>
+    <t>12.2%</t>
+  </si>
+  <si>
+    <t>1.94%</t>
+  </si>
+  <si>
+    <t>15.0%</t>
+  </si>
+  <si>
+    <t>8.70%</t>
+  </si>
+  <si>
+    <t>11.1%-13.3%</t>
+  </si>
+  <si>
+    <t>1.57%-2.40%</t>
+  </si>
+  <si>
+    <t>14.1%-16.0%</t>
+  </si>
+  <si>
+    <t>7.86%-9.62%</t>
+  </si>
+  <si>
+    <t>1.69%-3.57%</t>
+  </si>
+  <si>
+    <t>2.46%†</t>
+  </si>
+  <si>
+    <t>40.1%†</t>
+  </si>
+  <si>
+    <t>32.0%-48.7%</t>
+  </si>
+  <si>
+    <t>6.19% †</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.45%-8.53% </t>
+  </si>
+  <si>
+    <t>17.1%-20.1%</t>
+  </si>
+  <si>
+    <t>13.5% †</t>
+  </si>
+  <si>
+    <t>10.6%-16.9%</t>
+  </si>
+  <si>
+    <t>7.87%-9.51%</t>
   </si>
 </sst>
 </file>
@@ -411,15 +441,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -512,6 +533,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -522,60 +554,62 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6262,7 +6296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1EC72F-850F-44B2-9841-44FC67F38D52}">
   <dimension ref="B6:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -9234,213 +9268,243 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB7BBAE-5C34-40A0-8D10-B4B5B6A9B071}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>33</v>
+      <c r="A1" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>30</v>
+      <c r="B2" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>40</v>
+      <c r="A3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>109</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>32</v>
+      <c r="A4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>107</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>111</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="B18" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="C18" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="17" t="s">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="E22" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -9468,276 +9532,276 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="17">
+        <v>1993</v>
+      </c>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="19">
+        <v>1996</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="19">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="19">
+        <v>2003</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="19">
+        <v>2005</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="19">
+        <v>2009</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="19">
+        <v>2012</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="19">
+        <v>2014</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="19">
+        <v>2017</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="21">
-        <v>1993</v>
-      </c>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="23">
-        <v>1996</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="23">
-        <v>2000</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="23">
-        <v>2003</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B6" s="23">
-        <v>2005</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B7" s="23">
-        <v>2009</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="23">
-        <v>2012</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="23">
-        <v>2014</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="23">
-        <v>2017</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="N14" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q14" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="17">
+        <v>1988</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="J15" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="K14" s="27" t="s">
+      <c r="K15" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q15" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="19">
+        <v>1992</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="O16" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="P16" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q16" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="19">
+        <v>1996</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="P17" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q17" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="19">
+        <v>2000</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="M18" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="O18" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="P18" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q18" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="M14" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="N14" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="O14" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="P14" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q14" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="21">
-        <v>1988</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="J15" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="K15" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="L15" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="M15" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="N15" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="O15" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="P15" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q15" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="23">
-        <v>1992</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="L16" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="M16" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="N16" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="O16" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="P16" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q16" s="27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="23">
-        <v>1996</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="J17" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="K17" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="L17" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="M17" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="N17" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="O17" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="P17" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q17" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="23">
-        <v>2000</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="J18" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="K18" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="M18" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="N18" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="O18" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="P18" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q18" s="27" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="23">
+      <c r="B19" s="19">
         <v>2004</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>77</v>
+      <c r="C19" s="21" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="23">
+      <c r="B20" s="19">
         <v>2008</v>
       </c>
-      <c r="C20" s="25" t="s">
-        <v>78</v>
+      <c r="C20" s="21" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="23">
+      <c r="B21" s="19">
         <v>2012</v>
       </c>
-      <c r="C21" s="25" t="s">
-        <v>79</v>
+      <c r="C21" s="21" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="23">
+      <c r="B22" s="19">
         <v>2016</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>80</v>
+      <c r="C22" s="21" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>